<commit_message>
Updated for launcPage test case
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>PlatformName</t>
   </si>
@@ -54,30 +54,77 @@
     <t>Actual Pass Result</t>
   </si>
   <si>
-    <t>ActualFail Result</t>
-  </si>
-  <si>
-    <t>Page should open</t>
-  </si>
-  <si>
-    <t>Page opened.</t>
-  </si>
-  <si>
-    <t>Error!</t>
-  </si>
-  <si>
-    <t>Open Swiggy HomePage</t>
-  </si>
-  <si>
     <t>swiggy</t>
+  </si>
+  <si>
+    <t>Launch URL https://www.swiggy.com/</t>
+  </si>
+  <si>
+    <t>Swiggy Home Page should open.</t>
+  </si>
+  <si>
+    <t>Swiggy Home Page opened successfully</t>
+  </si>
+  <si>
+    <t>Problem loading swiggy home page.</t>
+  </si>
+  <si>
+    <t>Actual Fail Result</t>
+  </si>
+  <si>
+    <t>Verify that the login and signup links are present
+ on the homepage.</t>
+  </si>
+  <si>
+    <t>Login and signp links should be present.</t>
+  </si>
+  <si>
+    <t>Login and signup links are present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the input box for entering delivery 
+location is present along with Locate Me and 
+Find Food buttons. </t>
+  </si>
+  <si>
+    <t>Input box for entering delivery location is present along with Locate Me and Find Food buttons</t>
+  </si>
+  <si>
+    <t>Input box for entering delivery location should be present along with Locate Me and Find Food buttons.</t>
+  </si>
+  <si>
+    <t>Problem finding the login and signup links on the homepage.</t>
+  </si>
+  <si>
+    <t>Problem finding the Input box along with Locate Me and Find Food buttons.</t>
+  </si>
+  <si>
+    <t>Verify that text can be entered in the inputbox fordelivery location.</t>
+  </si>
+  <si>
+    <t>Text should be entered in the input box for delivery location.</t>
+  </si>
+  <si>
+    <t>Text  entered in the input box for delivery location.</t>
+  </si>
+  <si>
+    <t>Problem entering text in the input box for delivery location.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,8 +152,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -472,7 +523,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -482,49 +533,92 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for 2 test cases
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="3660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
     <sheet name="SetupTests" sheetId="2" r:id="rId2"/>
     <sheet name="LaunchPage" sheetId="3" r:id="rId3"/>
     <sheet name="LaunchPageScript" sheetId="4" r:id="rId4"/>
+    <sheet name="Login" sheetId="5" r:id="rId5"/>
+    <sheet name="LoginScript" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>PlatformName</t>
   </si>
@@ -42,9 +44,6 @@
     <t>launchPage</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -52,9 +51,6 @@
   </si>
   <si>
     <t>Actual Pass Result</t>
-  </si>
-  <si>
-    <t>swiggy</t>
   </si>
   <si>
     <t>Launch URL https://www.swiggy.com/</t>
@@ -99,9 +95,6 @@
     <t>Problem finding the Input box along with Locate Me and Find Food buttons.</t>
   </si>
   <si>
-    <t>Verify that text can be entered in the inputbox fordelivery location.</t>
-  </si>
-  <si>
     <t>Text should be entered in the input box for delivery location.</t>
   </si>
   <si>
@@ -109,6 +102,136 @@
   </si>
   <si>
     <t>Problem entering text in the input box for delivery location.</t>
+  </si>
+  <si>
+    <t>DeliveryLocation</t>
+  </si>
+  <si>
+    <t>Jodhpur, Rajasthan</t>
+  </si>
+  <si>
+    <t>Verify that text can be entered in the inputbox for delivery location.</t>
+  </si>
+  <si>
+    <t>Verify that the GooglePlayStore link is displayed on the homepage.</t>
+  </si>
+  <si>
+    <t>Verify the the AppStore link is displayed on the homepage.</t>
+  </si>
+  <si>
+    <t>GooglePlayStore link should be displayed on the homepage.</t>
+  </si>
+  <si>
+    <t>GooglePlayStore link is displayed on the homepage.</t>
+  </si>
+  <si>
+    <t>Problem finding the GooglePlayStore link.</t>
+  </si>
+  <si>
+    <t>AppStore link should be displayed on the homepage.</t>
+  </si>
+  <si>
+    <t>AppStore link is displayed on the homepage.</t>
+  </si>
+  <si>
+    <t>Problem finding the AppStore link.</t>
+  </si>
+  <si>
+    <t>Click on the GooglePlayStore link.</t>
+  </si>
+  <si>
+    <t>A new tab should open with GooglePlayStore page for downloading Swiggy.</t>
+  </si>
+  <si>
+    <t>A new tab opened with GooglePlayStore page for downloading Swiggy.</t>
+  </si>
+  <si>
+    <t>Problem loading the GooglePlayStore page for Swiggy.</t>
+  </si>
+  <si>
+    <t>Click on the AppStore link.</t>
+  </si>
+  <si>
+    <t>A new tab should open with AppStore page for downloading Swiggy.</t>
+  </si>
+  <si>
+    <t>A new tab opened with AppStore page for downloading Swiggy.</t>
+  </si>
+  <si>
+    <t>Problem loading the AppStore page for Swiggy.</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>Verify that the login link is present
+ on the homepage.</t>
+  </si>
+  <si>
+    <t>Login link should be present.</t>
+  </si>
+  <si>
+    <t>Login link is present.</t>
+  </si>
+  <si>
+    <t>Problem finding the login link on the homepage.</t>
+  </si>
+  <si>
+    <t>Click on the login link.</t>
+  </si>
+  <si>
+    <t>A new form should appear for Login.</t>
+  </si>
+  <si>
+    <t>Login form appeared.</t>
+  </si>
+  <si>
+    <t>Problem loading the form for Login.</t>
+  </si>
+  <si>
+    <t>Enter the ten digit phone no in the Phone no field.</t>
+  </si>
+  <si>
+    <t>Phone number should be entered.</t>
+  </si>
+  <si>
+    <t>Phone number is entered.</t>
+  </si>
+  <si>
+    <t>Problem entering phone number.</t>
+  </si>
+  <si>
+    <t>Click on login button.</t>
+  </si>
+  <si>
+    <t>OTP field should be displayed.</t>
+  </si>
+  <si>
+    <t>OTP field is displayed.</t>
+  </si>
+  <si>
+    <t>Problem loading the OTP field.</t>
+  </si>
+  <si>
+    <t>Enter random number in OTP field and click Verify OTP.</t>
+  </si>
+  <si>
+    <t>Enter Valid OTP warning should appear.</t>
+  </si>
+  <si>
+    <t>Enter Valid OTP warning appears.</t>
+  </si>
+  <si>
+    <t>Problem loading the warning.</t>
+  </si>
+  <si>
+    <t>RandomOTP</t>
+  </si>
+  <si>
+    <t>123f</t>
   </si>
 </sst>
 </file>
@@ -152,12 +275,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,9 +604,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -491,13 +615,19 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -515,15 +645,18 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -533,10 +666,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,76 +682,287 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>7792016995</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to run 3 test cases
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="3660" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="3660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,10 @@
     <sheet name="LaunchPageScript" sheetId="4" r:id="rId4"/>
     <sheet name="Login" sheetId="5" r:id="rId5"/>
     <sheet name="LoginScript" sheetId="6" r:id="rId6"/>
+    <sheet name="AddToCart" sheetId="7" r:id="rId7"/>
+    <sheet name="AddToCartScript" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
   <si>
     <t>PlatformName</t>
   </si>
@@ -236,6 +237,87 @@
   </si>
   <si>
     <t>7792016995</t>
+  </si>
+  <si>
+    <t>Restaurants page should be loaded.</t>
+  </si>
+  <si>
+    <t>Restaurants page is loaded.</t>
+  </si>
+  <si>
+    <t>Problem redirecting to the Restaurant page.</t>
+  </si>
+  <si>
+    <t>Enter the delivery location.</t>
+  </si>
+  <si>
+    <t>Verify the delivery location city.</t>
+  </si>
+  <si>
+    <t>Delivery Location City should match the City given as test data.</t>
+  </si>
+  <si>
+    <t>Delivery Location City matches the City given as test data.</t>
+  </si>
+  <si>
+    <t>Incorrect Delivery location found.</t>
+  </si>
+  <si>
+    <t>Click on the Search button.</t>
+  </si>
+  <si>
+    <t>User should be redirected to Search Page and a search box should be present.</t>
+  </si>
+  <si>
+    <t>User is redirected to Search Page and a search box is present.</t>
+  </si>
+  <si>
+    <t>Problem loading the Search page correctly.</t>
+  </si>
+  <si>
+    <t>addToCart</t>
+  </si>
+  <si>
+    <t>Search for the dish to be ordered.</t>
+  </si>
+  <si>
+    <t>Dish</t>
+  </si>
+  <si>
+    <t>Cake</t>
+  </si>
+  <si>
+    <t>By default a list for restairants should be shown.</t>
+  </si>
+  <si>
+    <t>By default a list for restaurants is shown.</t>
+  </si>
+  <si>
+    <t>Problem loadin the search results for the dish.</t>
+  </si>
+  <si>
+    <t>Go to Dishes Tab and Add the first Dish to the cart.</t>
+  </si>
+  <si>
+    <t>A popup should appear for customizing the dish.</t>
+  </si>
+  <si>
+    <t>Popup appeared for customizing the dish.</t>
+  </si>
+  <si>
+    <t>Problem loading the popup.</t>
+  </si>
+  <si>
+    <t>Click on Add Item button.</t>
+  </si>
+  <si>
+    <t>Item should be added to the cart.</t>
+  </si>
+  <si>
+    <t>Item is added to the cart.</t>
+  </si>
+  <si>
+    <t>Problem adding item to the cart.</t>
   </si>
 </sst>
 </file>
@@ -279,13 +361,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,9 +693,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -619,19 +704,25 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
       <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -645,7 +736,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +764,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -969,4 +1060,171 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>